<commit_message>
still problem with parse str to dict from setting1.xlsx ; should try write parse value to settings or check limit of len in one cell excell2
</commit_message>
<xml_diff>
--- a/setting1.xlsx
+++ b/setting1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
   <si>
     <t>number</t>
   </si>
@@ -131,6 +131,54 @@
     <t>{"getToken": {"error": 0, "values": {"token": "6C08AD5F0D1A3A883545FED46A6F80BE","pukResponse":"","pukCnt":"","roleLic":"Contract Administrator","roleValue":"Администратор «Абонент»","roleDes":"Роль «Администратор «Абонент» предоставляет возможность управлять услугами и сервисами всех номеров на всех лицевых счетах контракта","roleOrder":"5","calcMethod":"PoP","billNumber":"295405598213","rtmAccessToken":"eyJhbGciOiJSUzI1NiIsInR5cCI6IkpXVCJ9.eyJzY29wZSI6WyJtc191YWFfY3JlZGVudGlhbF90eXBlX3Bhc3N3b3JkX2p3dCIsInRtZl9tc19yZXNvdXJjZV9wcm9maWxlOlZBTElEQVRFLUlNRUkiLCJ0bWZfbXNfaW50ZXJhY3Rpb25fcHJvZmlsZTpSVE0tVEVDSE5JQ0FMIiwidG1mX21zX2ludGVyYWN0aW9uX3Byb2ZpbGU6UlRNIiwib3BlbmlkIiwidG1mX21zX2FjdGl2YXRpb25fc2VydmljZV90eXBlOkREUy1TWU5DLUFDVElWQVRJT04iLCJ0bWZfbXNfcmVzb3VyY2VfcHJvZmlsZTpBTlRJRlJBVUQtU0lNLUNIQU5HRSIsInRtZl9tc19xdWFsaWZpY2F0aW9uX3Byb2ZpbGU6UlRNOkNSTSIsInRtZl9tc19hY3RpdmF0aW9uX3NlcnZpY2VfdHlwZTpERFMtU1lOQy1ERUFDVElWQVRJT04iXSwiZXhwIjoxNjE1ODE0ODAxLCJhZGRpdGlvbmFsRGV0YWlscyI6eyJtc2lzZG4iOiIzODA5NTIyNDAwMTYifSwiYXV0aG9yaXRpZXMiOlsiUk9MRV9TWVNURU0iXSwianRpIjoiY2E5YTlkMGUtOWIwOC00YTJmLWFjMGYtMjE2ZDkzZDZmYTQ4IiwidGVuYW50IjoiWE0iLCJjbGllbnRfaWQiOiJzdmMtY3JtLW13In0.WfZlUix0QG1gV5L802wklpYbYsV-YeL2I8s5TvUyIaP5KPlgpzYrGJ_rv4WGBPNIFAlESo8awGfkcposMnBKjgqcNJcFh-DGFD6QAPOuvO6j7hn8sgo038JIqYBLvaQeOPCaV3_nJX92S29Y1Cv4D1cCuRjzwpHP5oq6jXk2AlSb-yioJqUzCvTh30k4TeggZl39XOeRqvhcRjPNufJSfS_RNM7B5hr-VvBfNao2GKPIQ4S7dg1-i7w0h_An1PFBPY_js_lfyh3atjudFFb7_cbx3Q5MMo7JT8nS17o6ebl4aca_jnAOfHlvyOiCzy9Ev4qOwJkYEYg7o285QMJzDQ","rtmRefreshToken":"","pin":true,"isShowedPin":false}},"identification": {"error": 0, "values": { "id":""}}}</t>
   </si>
   <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"settings":{}}}</t>
+  </si>
+  <si>
+    <t>getMark</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"getMarkCatByMSISDN":{"identificator":"952240016"}}}</t>
+  </si>
+  <si>
+    <t>getAccessRole</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"getAccessRoleCorpMSISDN":{"msisdn":"952240016"}}}</t>
+  </si>
+  <si>
+    <t>getRelPhone</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"getRelPhone":{}}}</t>
+  </si>
+  <si>
+    <t>getLinks</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"getLinks":{}}}</t>
+  </si>
+  <si>
+    <t>countersMain</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"countersMainV2":{}}}</t>
+  </si>
+  <si>
+    <t>currentPlan</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"currentPlan":{}}}</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>{"params":{"version":"2.1.2","language":"ru","source":"WebApp","token":"1C43EFEA009159BC503AFF3E5F5E32FD","manufacture":"","childNumber":"","accessType":"","spinner":1},"requests":{"balance":{}}}</t>
+  </si>
+  <si>
     <t>начальная точка</t>
   </si>
   <si>
@@ -273,6 +321,24 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>подстановка значений</t>
+  </si>
+  <si>
+    <t>token_siebel</t>
+  </si>
+  <si>
+    <t>{{token_siebel}}</t>
+  </si>
+  <si>
+    <t>gerRelPhone</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>{{phone}}</t>
   </si>
 </sst>
 </file>
@@ -280,10 +346,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -309,14 +375,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -329,30 +411,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,22 +459,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -415,7 +467,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,6 +495,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -446,187 +512,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,17 +736,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -730,25 +790,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -767,59 +824,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -828,91 +894,91 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1273,10 +1339,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1463,7 +1529,7 @@
     </row>
     <row r="18" ht="259.2" spans="1:9">
       <c r="A18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1489,6 +1555,276 @@
       <c r="I18" s="3" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="20" ht="57.6" spans="1:8">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" ht="57.6" spans="1:8">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" ht="57.6" spans="1:8">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" ht="57.6" spans="1:8">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" ht="57.6" spans="1:8">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" ht="57.6" spans="1:8">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" ht="57.6" spans="1:8">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" ht="57.6" spans="1:8">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7">
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="6:7">
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="6:7">
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" ht="57.6" spans="1:8">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H41">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7">
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="6:7">
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="6:7">
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="6:7">
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="6:7">
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="6:7">
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1499,10 +1835,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1519,23 +1855,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -1543,147 +1879,147 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1691,7 +2027,7 @@
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1">
         <v>50</v>
@@ -1699,7 +2035,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1">
         <v>51</v>
@@ -1707,7 +2043,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1">
         <v>52</v>
@@ -1715,7 +2051,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1">
         <v>53</v>
@@ -1723,7 +2059,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1">
         <v>54</v>
@@ -1731,7 +2067,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1">
         <v>55</v>
@@ -1739,7 +2075,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1">
         <v>56</v>
@@ -1747,7 +2083,7 @@
     </row>
     <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C23" s="1">
         <v>57</v>
@@ -1755,7 +2091,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C24" s="1">
         <v>58</v>
@@ -1763,7 +2099,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1">
         <v>59</v>
@@ -1771,20 +2107,62 @@
     </row>
     <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:3">
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:3">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="3:3">
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
       <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>